<commit_message>
Added functionality for testing tracking consistency by calculating tvec and rvec standard deviation in MainActivity. Updated test data spreadsheet.
</commit_message>
<xml_diff>
--- a/fps_benchmark_results.xlsx
+++ b/fps_benchmark_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t>Resolution</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Trial #1 (FPS)</t>
-  </si>
-  <si>
-    <t>Average</t>
   </si>
   <si>
     <t>1280 x 720</t>
@@ -56,15 +53,92 @@
     <t>256 x 144</t>
   </si>
   <si>
-    <t>Max Distance</t>
+    <t>Max Distance (cm)</t>
+  </si>
+  <si>
+    <t>Average FPS</t>
+  </si>
+  <si>
+    <t>Trial #1 (m)</t>
+  </si>
+  <si>
+    <t>Average Std Dev</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Accuracy (std dev of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rvec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for stationary marker and camera)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Accuracy (std dev of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tvec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for stationary marker and camera)</t>
+    </r>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -116,10 +190,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -129,7 +203,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -307,11 +391,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="312214088"/>
-        <c:axId val="371400872"/>
+        <c:axId val="314675920"/>
+        <c:axId val="314677488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="312214088"/>
+        <c:axId val="314675920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +452,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371400872"/>
+        <c:crossAx val="314677488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -377,7 +461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="371400872"/>
+        <c:axId val="314677488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -434,7 +518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312214088"/>
+        <c:crossAx val="314675920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -446,6 +530,1373 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Max Distance (cm) vs. Processing Resolution</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max Distance (cm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256 x 144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280 x 720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1920 x 1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048 x 1152</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3264 x 1836</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="378611160"/>
+        <c:axId val="378608024"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="378611160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378608024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378608024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378611160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Standard Deviation of Tvec</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Resolution</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18943066491688543"/>
+          <c:y val="5.0925925925925923E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>x</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256 x 144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280 x 720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1920 x 1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048 x 1152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$27:$K$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.4047489613412729E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6061295030178106E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0252883304974932E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1393488780255264E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256 x 144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280 x 720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1920 x 1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048 x 1152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$27:$L$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.7687367433012705E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7082970405507998E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2076794494100567E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0774975330886E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256 x 144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280 x 720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1920 x 1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048 x 1152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$27:$M$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.4332991763647774E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3424174291514766E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8350042634447367E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5884700251884866E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="378604888"/>
+        <c:axId val="378606064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="378604888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378606064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378606064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378604888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Standard</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Deviation of Rvec Quaternions</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Resolution</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>w</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$36:$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256 x 144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280 x 720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1920 x 1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048 x 1152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$36:$N$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.7147047027750204E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6711188692572109E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6545016659618335E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5861675845114968E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>x</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$36:$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256 x 144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280 x 720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1920 x 1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048 x 1152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$36:$O$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.4317223925952467E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2678001955308325E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3634798319716265E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6074213114232496E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$36:$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256 x 144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280 x 720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1920 x 1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048 x 1152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$36:$P$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.7853971627889396E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1211811689380389E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7428530212531698E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5017726445309263E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$36:$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256 x 144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280 x 720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1920 x 1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048 x 1152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$36:$Q$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.705615675646196E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9397298643114258E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2249219194080136E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2310449237840837E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="312982096"/>
+        <c:axId val="312982488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="312982096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="312982488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="312982488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="312982096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -523,6 +1974,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1039,20 +2610,1568 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1066,6 +4185,96 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1337,21 +4546,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1368,16 +4579,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>50.7612308785354</v>
@@ -1388,7 +4599,9 @@
       <c r="D2" s="2">
         <v>61.939307172166998</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <v>53</v>
+      </c>
       <c r="F2" s="2">
         <f>AVERAGE(B2:D2)</f>
         <v>56.068078749313969</v>
@@ -1397,7 +4610,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>5.7141219353375501</v>
@@ -1408,16 +4621,18 @@
       <c r="D3" s="2">
         <v>7.8983451762417403</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2">
+        <v>55</v>
+      </c>
       <c r="F3" s="2">
-        <f>AVERAGE(B3:D3)</f>
+        <f t="shared" ref="F3:F6" si="0">AVERAGE(B3:D3)</f>
         <v>6.3951976206339038</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>3.0380554161316402</v>
@@ -1428,16 +4643,18 @@
       <c r="D4" s="2">
         <v>3.5644915999412201</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>53.5</v>
+      </c>
       <c r="F4" s="2">
-        <f>AVERAGE(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>3.4718758029214167</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>2.9230053472626998</v>
@@ -1448,16 +4665,18 @@
       <c r="D5" s="2">
         <v>3.2968860900192198</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>55</v>
+      </c>
       <c r="F5" s="2">
-        <f>AVERAGE(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>3.3696185327372699</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="8">
         <v>1.0328774780576</v>
@@ -1468,9 +4687,11 @@
       <c r="D6" s="8">
         <v>1.2926021557304299</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8">
+        <v>56</v>
+      </c>
       <c r="F6" s="2">
-        <f>AVERAGE(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>1.1997998325790966</v>
       </c>
       <c r="G6" s="5"/>
@@ -1480,6 +4701,612 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
     </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="10">
+        <v>6.5192580223083496E-9</v>
+      </c>
+      <c r="C27" s="10">
+        <v>9.3132257461547802E-9</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1.4901161193847601E-7</v>
+      </c>
+      <c r="E27" s="10">
+        <v>7.21312929693428E-5</v>
+      </c>
+      <c r="F27" s="10">
+        <v>2.62875837784115E-5</v>
+      </c>
+      <c r="G27" s="10">
+        <v>2.52835062517811E-4</v>
+      </c>
+      <c r="H27" s="10">
+        <v>4.6566128730773901E-9</v>
+      </c>
+      <c r="I27" s="10">
+        <v>9.3132257461547802E-9</v>
+      </c>
+      <c r="J27" s="10">
+        <v>1.49011611938476E-8</v>
+      </c>
+      <c r="K27" s="10">
+        <f>AVERAGE(B27,E27,H27)</f>
+        <v>2.4047489613412729E-5</v>
+      </c>
+      <c r="L27" s="10">
+        <f t="shared" ref="L27:M31" si="1">AVERAGE(C27,F27,I27)</f>
+        <v>8.7687367433012705E-6</v>
+      </c>
+      <c r="M27" s="10">
+        <f t="shared" si="1"/>
+        <v>8.4332991763647774E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="10">
+        <v>7.06449201171696E-5</v>
+      </c>
+      <c r="C28" s="10">
+        <v>6.9527470434186195E-5</v>
+      </c>
+      <c r="D28" s="10">
+        <v>3.6030516234579799E-4</v>
+      </c>
+      <c r="E28" s="10">
+        <v>4.3885566655424702E-5</v>
+      </c>
+      <c r="F28" s="10">
+        <v>3.0411772360215E-5</v>
+      </c>
+      <c r="G28" s="10">
+        <v>1.6943629647016899E-4</v>
+      </c>
+      <c r="H28" s="10">
+        <v>1.1365339831794E-4</v>
+      </c>
+      <c r="I28" s="10">
+        <v>7.1309668422122805E-5</v>
+      </c>
+      <c r="J28" s="10">
+        <v>1.72983769929476E-4</v>
+      </c>
+      <c r="K28" s="10">
+        <f t="shared" ref="K28:K31" si="2">AVERAGE(B28,E28,H28)</f>
+        <v>7.6061295030178106E-5</v>
+      </c>
+      <c r="L28" s="10">
+        <f t="shared" si="1"/>
+        <v>5.7082970405507998E-5</v>
+      </c>
+      <c r="M28" s="10">
+        <f t="shared" si="1"/>
+        <v>2.3424174291514766E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="10">
+        <v>2.6571997989634498E-4</v>
+      </c>
+      <c r="C29" s="10">
+        <v>1.2983339933212901E-4</v>
+      </c>
+      <c r="D29" s="10">
+        <v>3.7522038065353398E-4</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1.5410759294070899E-4</v>
+      </c>
+      <c r="F29" s="10">
+        <v>1.0556371308508599E-4</v>
+      </c>
+      <c r="G29" s="10">
+        <v>2.4164280216903901E-4</v>
+      </c>
+      <c r="H29" s="10">
+        <v>1.87758926312194E-4</v>
+      </c>
+      <c r="I29" s="10">
+        <v>1.2690672240580199E-4</v>
+      </c>
+      <c r="J29" s="10">
+        <v>2.3363809621084801E-4</v>
+      </c>
+      <c r="K29" s="10">
+        <f t="shared" si="2"/>
+        <v>2.0252883304974932E-4</v>
+      </c>
+      <c r="L29" s="10">
+        <f t="shared" si="1"/>
+        <v>1.2076794494100567E-4</v>
+      </c>
+      <c r="M29" s="10">
+        <f t="shared" si="1"/>
+        <v>2.8350042634447367E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="10">
+        <v>2.38617061906858E-4</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1.8841680628876899E-4</v>
+      </c>
+      <c r="D30" s="10">
+        <v>4.60917025780932E-4</v>
+      </c>
+      <c r="E30" s="10">
+        <v>3.5984464883688798E-4</v>
+      </c>
+      <c r="F30" s="10">
+        <v>2.2891602068417E-4</v>
+      </c>
+      <c r="G30" s="10">
+        <v>2.9955841669436403E-4</v>
+      </c>
+      <c r="H30" s="10">
+        <v>3.4334295266391201E-4</v>
+      </c>
+      <c r="I30" s="10">
+        <v>2.0591643295364101E-4</v>
+      </c>
+      <c r="J30" s="10">
+        <v>3.1606556508125E-4</v>
+      </c>
+      <c r="K30" s="10">
+        <f t="shared" si="2"/>
+        <v>3.1393488780255264E-4</v>
+      </c>
+      <c r="L30" s="10">
+        <f t="shared" si="1"/>
+        <v>2.0774975330886E-4</v>
+      </c>
+      <c r="M30" s="10">
+        <f t="shared" si="1"/>
+        <v>3.5884700251884866E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L31" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P35" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="10">
+        <v>7.7715611723760899E-16</v>
+      </c>
+      <c r="C36" s="10">
+        <v>1.6653345369377299E-16</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1.6653345369377299E-16</v>
+      </c>
+      <c r="E36" s="10">
+        <v>1.33226762955018E-15</v>
+      </c>
+      <c r="F36" s="10">
+        <v>5.1441141083172898E-4</v>
+      </c>
+      <c r="G36" s="10">
+        <v>1.02951671777813E-3</v>
+      </c>
+      <c r="H36" s="10">
+        <v>5.35619148835988E-4</v>
+      </c>
+      <c r="I36" s="10">
+        <v>8.1168470267498505E-5</v>
+      </c>
+      <c r="J36" s="10">
+        <v>0</v>
+      </c>
+      <c r="K36" s="10">
+        <v>2.7755575615628899E-16</v>
+      </c>
+      <c r="L36" s="10">
+        <v>5.2735593669694896E-16</v>
+      </c>
+      <c r="M36" s="10">
+        <v>5.5511151231257797E-16</v>
+      </c>
+      <c r="N36" s="10">
+        <f>AVERAGE(B36,F36,J36)</f>
+        <v>1.7147047027750204E-4</v>
+      </c>
+      <c r="O36" s="10">
+        <f t="shared" ref="O36:Q40" si="3">AVERAGE(C36,G36,K36)</f>
+        <v>3.4317223925952467E-4</v>
+      </c>
+      <c r="P36" s="10">
+        <f t="shared" si="3"/>
+        <v>1.7853971627889396E-4</v>
+      </c>
+      <c r="Q36" s="10">
+        <f t="shared" si="3"/>
+        <v>2.705615675646196E-5</v>
+      </c>
+      <c r="R36" s="10"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="10">
+        <v>8.0396829864335295E-4</v>
+      </c>
+      <c r="C37" s="12">
+        <v>1.38992803753456E-3</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1.20833339026588E-3</v>
+      </c>
+      <c r="E37" s="10">
+        <v>7.2075735445311403E-4</v>
+      </c>
+      <c r="F37" s="10">
+        <v>8.0623360764570497E-5</v>
+      </c>
+      <c r="G37" s="10">
+        <v>8.7415753971097803E-4</v>
+      </c>
+      <c r="H37" s="10">
+        <v>6.4240335907977703E-4</v>
+      </c>
+      <c r="I37" s="10">
+        <v>3.6980250199202398E-4</v>
+      </c>
+      <c r="J37" s="10">
+        <v>1.11674400136924E-3</v>
+      </c>
+      <c r="K37" s="10">
+        <v>1.5393150093469599E-3</v>
+      </c>
+      <c r="L37" s="10">
+        <v>1.5128067574684599E-3</v>
+      </c>
+      <c r="M37" s="10">
+        <v>1.89135910284829E-3</v>
+      </c>
+      <c r="N37" s="10">
+        <f t="shared" ref="N37:N40" si="4">AVERAGE(B37,F37,J37)</f>
+        <v>6.6711188692572109E-4</v>
+      </c>
+      <c r="O37" s="10">
+        <f t="shared" si="3"/>
+        <v>1.2678001955308325E-3</v>
+      </c>
+      <c r="P37" s="10">
+        <f t="shared" si="3"/>
+        <v>1.1211811689380389E-3</v>
+      </c>
+      <c r="Q37" s="10">
+        <f t="shared" si="3"/>
+        <v>9.9397298643114258E-4</v>
+      </c>
+      <c r="R37" s="10"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="10">
+        <v>1.8832830206164199E-3</v>
+      </c>
+      <c r="C38" s="10">
+        <v>3.8336513107247198E-3</v>
+      </c>
+      <c r="D38" s="10">
+        <v>3.0424228465441498E-3</v>
+      </c>
+      <c r="E38" s="10">
+        <v>3.6408473975771401E-3</v>
+      </c>
+      <c r="F38" s="10">
+        <v>1.40236231548935E-3</v>
+      </c>
+      <c r="G38" s="10">
+        <v>2.9563062153167901E-3</v>
+      </c>
+      <c r="H38" s="10">
+        <v>2.3808205825510999E-3</v>
+      </c>
+      <c r="I38" s="10">
+        <v>2.76660835220047E-3</v>
+      </c>
+      <c r="J38" s="10">
+        <v>1.6778596617797301E-3</v>
+      </c>
+      <c r="K38" s="10">
+        <v>3.3004819698733701E-3</v>
+      </c>
+      <c r="L38" s="10">
+        <v>2.80531563466426E-3</v>
+      </c>
+      <c r="M38" s="10">
+        <v>3.26731000844643E-3</v>
+      </c>
+      <c r="N38" s="10">
+        <f t="shared" si="4"/>
+        <v>1.6545016659618335E-3</v>
+      </c>
+      <c r="O38" s="10">
+        <f t="shared" si="3"/>
+        <v>3.3634798319716265E-3</v>
+      </c>
+      <c r="P38" s="10">
+        <f t="shared" si="3"/>
+        <v>2.7428530212531698E-3</v>
+      </c>
+      <c r="Q38" s="10">
+        <f t="shared" si="3"/>
+        <v>3.2249219194080136E-3</v>
+      </c>
+      <c r="R38" s="10"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="10">
+        <v>1.94644236144333E-3</v>
+      </c>
+      <c r="C39" s="10">
+        <v>4.4347771005581599E-3</v>
+      </c>
+      <c r="D39" s="10">
+        <v>3.5904977737683899E-3</v>
+      </c>
+      <c r="E39" s="10">
+        <v>4.0264276222710203E-3</v>
+      </c>
+      <c r="F39" s="10">
+        <v>3.1025808888649701E-3</v>
+      </c>
+      <c r="G39" s="10">
+        <v>6.6577243242267404E-3</v>
+      </c>
+      <c r="H39" s="10">
+        <v>5.3034390633159697E-3</v>
+      </c>
+      <c r="I39" s="10">
+        <v>6.2448289693880204E-3</v>
+      </c>
+      <c r="J39" s="10">
+        <v>2.7094795032261902E-3</v>
+      </c>
+      <c r="K39" s="10">
+        <v>5.7297625094848504E-3</v>
+      </c>
+      <c r="L39" s="10">
+        <v>4.6113810965084196E-3</v>
+      </c>
+      <c r="M39" s="10">
+        <v>5.4218781796932097E-3</v>
+      </c>
+      <c r="N39" s="10">
+        <f t="shared" si="4"/>
+        <v>2.5861675845114968E-3</v>
+      </c>
+      <c r="O39" s="10">
+        <f t="shared" si="3"/>
+        <v>5.6074213114232496E-3</v>
+      </c>
+      <c r="P39" s="10">
+        <f t="shared" si="3"/>
+        <v>4.5017726445309263E-3</v>
+      </c>
+      <c r="Q39" s="10">
+        <f t="shared" si="3"/>
+        <v>5.2310449237840837E-3</v>
+      </c>
+      <c r="R39" s="10"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O40" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P40" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q40" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>